<commit_message>
Support for negative values and bookmarks Bug fix for 0 values
</commit_message>
<xml_diff>
--- a/documents/Published/Ring Chart/RingChartbyMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Ring Chart/RingChartbyMAQSoftwareChecklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Power BI\RingChart\17-10-17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI-CustomVisuals\documents\Published\Ring Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CEEC5B-7D35-4346-A5DA-E7AD7DE130CB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15285" windowHeight="5310" xr2:uid="{298230A1-4D6D-45FE-9FCF-FFB948C6A0D6}"/>
   </bookViews>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="133">
   <si>
     <r>
       <t>#</t>
@@ -389,36 +390,16 @@
     <t xml:space="preserve">Secondary summary labels color should be changed to 'Black' and font size should be changed to '16'. </t>
   </si>
   <si>
-    <t>Donut title</t>
-  </si>
-  <si>
-    <t>1. Go to formatting pane
-2. Turn off 'Donut title'</t>
-  </si>
-  <si>
     <t>Title of the Ring chart should be hidden</t>
   </si>
   <si>
     <t>Check whether Title text and Tooltip text settings are working fine</t>
   </si>
   <si>
-    <t>1. Go to formatting pane
-2. Go to 'Donut title'
-3. Update the Title text to 'Ring chart'
-4. Update the Tooltip text to 'Ring chart custom visual tooltip'</t>
-  </si>
-  <si>
     <t>Title of the Ring chart should be updated to 'Ring chart' and on hover of the (?), 'Ring chart custom visual tooltip' should be displayed</t>
   </si>
   <si>
     <t>Check whether Font color, Text size and Background color settings are working fine</t>
-  </si>
-  <si>
-    <t>1. Go to formatting pane
-2. Go to 'Donut title'
-3. Update the Font color to 'Black'
-4. Update the Text size to '16'
-5. Update the background color to 'Yellow'</t>
   </si>
   <si>
     <t>Title color should be updated to 'Black', Text size should be updated to '16' and background color of Ring chart title should be changed to 'Yellow'</t>
@@ -525,6 +506,65 @@
   </si>
   <si>
     <t>Secondary measure summary value should display value in 'Thousands' and with 2 decimal places</t>
+  </si>
+  <si>
+    <t>Bookmarks</t>
+  </si>
+  <si>
+    <t>Check if Bookmarks feature working</t>
+  </si>
+  <si>
+    <t>1. Go to View -&gt; Turn on Bookmarks Pane
+2. Do some selections and filtering too if needed in visual
+3. In Bookmarks Pane, add a new bookmark and update it
+4. Change selections and click on the saved bookmark</t>
+  </si>
+  <si>
+    <t>1. Bookmarks Pane will be visible on the right side
+2. Visual will render according to selections
+3. A new entry of bookmark will be added in Bookmarks Pane, selection will be saved in it after update
+4. Saved selections will render in the visual on clicking the bookmark</t>
+  </si>
+  <si>
+    <t>Negative Value</t>
+  </si>
+  <si>
+    <t>Ring title</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Turn off 'Ring title'</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Ring title'
+3. Update the Title text to 'Ring chart'
+4. Update the Tooltip text to 'Ring chart custom visual tooltip'</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Ring title'
+3. Update the Font color to 'Black'
+4. Update the Text size to '16'
+5. Update the background color to 'Yellow'</t>
+  </si>
+  <si>
+    <t>Check whether chart is plotting for negative values and negative value arc settings is working</t>
+  </si>
+  <si>
+    <t>1. Select value column with negative data to 'Primary Measure' input field
+2. Go to formatting pane.
+3. In Negative value arc settings, set the arc position to normal.
+4. In Negative value arc settings, set the arc position to pop out.
+5. In Negative value arc settings, set the arc position to drop in.
+6. In Negative value arc settings, turn on Pattern fill toggle.</t>
+  </si>
+  <si>
+    <t>1. Plot should render for negative values also and data labels should also appear for the respective arc.
+2. Arc for negative values are positioned normally.
+3. Arc for negative values are poped outside the normal arc.
+4. Arc for negative values are dropped inside the normal arc.
+5. Arc for negative values are filled in line pattern.</t>
   </si>
 </sst>
 </file>
@@ -602,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -631,22 +671,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -962,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BD6B43-E3C6-4B92-AF1B-22928F3D0975}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +1026,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -991,7 +1040,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1005,8 +1054,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C3" t="s">
@@ -1017,8 +1066,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="16"/>
       <c r="C4" t="s">
         <v>38</v>
       </c>
@@ -1027,7 +1076,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="17" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1041,7 +1090,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="5" t="s">
         <v>44</v>
       </c>
@@ -1053,7 +1102,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1067,7 +1116,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="5" t="s">
         <v>51</v>
       </c>
@@ -1079,7 +1128,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="5" t="s">
         <v>54</v>
       </c>
@@ -1091,7 +1140,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="5" t="s">
         <v>57</v>
       </c>
@@ -1103,7 +1152,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="5" t="s">
         <v>60</v>
       </c>
@@ -1129,7 +1178,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1143,7 +1192,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="5" t="s">
         <v>73</v>
       </c>
@@ -1155,7 +1204,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="5" t="s">
         <v>72</v>
       </c>
@@ -1167,7 +1216,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="17" t="s">
         <v>76</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1181,7 +1230,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="5" t="s">
         <v>81</v>
       </c>
@@ -1193,7 +1242,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="5" t="s">
         <v>85</v>
       </c>
@@ -1205,171 +1254,199 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="18" t="s">
         <v>84</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>90</v>
+      <c r="A21" s="17" t="s">
+        <v>126</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="5" t="s">
+    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="5" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>99</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="5" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>108</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="5" t="s">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>115</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31" s="5" t="s">
+    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>121</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1580,29 +1657,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="19">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="19" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="19"/>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="13"/>
+      <c r="C19" s="19"/>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -1616,41 +1693,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="A21" s="19">
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="19" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="13"/>
+      <c r="C22" s="19"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="13"/>
+      <c r="C23" s="19"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="13"/>
+      <c r="C24" s="19"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2">

</xml_diff>